<commit_message>
Ouverture et fermeture System1
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\OneDrive - Positive Thinking Company\Documents\3 - UiPath\CalculateClientSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\OneDrive - Positive Thinking Company\Documents\UiPath\CalculateClientSecurityHash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29D10DE-FB62-4701-8F86-4EADC7659361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52A7D67-2F37-430A-9E38-357B14D02C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -137,13 +137,31 @@
   </si>
   <si>
     <t>Credential Asset of ACME System 1</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>TimeoutXS</t>
+  </si>
+  <si>
+    <t>TimeoutS</t>
+  </si>
+  <si>
+    <t>TimeoutM</t>
+  </si>
+  <si>
+    <t>TimeoutL</t>
+  </si>
+  <si>
+    <t>TimeoutXL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -167,6 +185,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -185,15 +209,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -509,7 +536,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -581,6 +608,9 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
         <v>31</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
@@ -1596,8 +1626,11 @@
     <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{71D58DCF-ACD5-4986-B4D2-3A197EA59735}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1606,7 +1639,7 @@
   <dimension ref="A1:Z987"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1731,11 +1764,46 @@
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>60000</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -2718,7 +2786,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Je viens de terminer navigateToWIID
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quentin\OneDrive - Positive Thinking Company\Documents\UiPath\CalculateClientSecurityHash\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://positivethinkingcompany-my.sharepoint.com/personal/qcacciatore_positivethinking_tech/Documents/Documents/UiPath/CalculateClientSecurityHash/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52A7D67-2F37-430A-9E38-357B14D02C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{2A6525FB-7BDA-4D0F-9164-6A03507BD645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ACA86652-2A24-4219-AA6D-88FE3D941E2B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
   <si>
     <t>Name</t>
   </si>
@@ -103,30 +103,12 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>System1 URL</t>
-  </si>
-  <si>
-    <t>SHA1 Online URL</t>
-  </si>
-  <si>
     <t>System1_Credential</t>
   </si>
   <si>
@@ -155,13 +137,22 @@
   </si>
   <si>
     <t>TimeoutXL</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>System1_URL</t>
+  </si>
+  <si>
+    <t>SHA1Online_URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -185,12 +176,6 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,18 +194,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -533,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -582,60 +564,53 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>35</v>
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1622,15 +1597,14 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{71D58DCF-ACD5-4986-B4D2-3A197EA59735}"/>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{71D58DCF-ACD5-4986-B4D2-3A197EA59735}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{F699C768-E7D6-471C-B7CF-E89689BEBBC5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1638,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1766,7 +1740,7 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>1000</v>
@@ -1774,7 +1748,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>5000</v>
@@ -1782,7 +1756,7 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B14">
         <v>10000</v>
@@ -1790,7 +1764,7 @@
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>30000</v>
@@ -1798,7 +1772,7 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>60000</v>

</xml_diff>